<commit_message>
Update the test datat from U7BM9E to G1S77A
</commit_message>
<xml_diff>
--- a/data/NGQ_US9409_10_data.xlsx
+++ b/data/NGQ_US9409_10_data.xlsx
@@ -57,9 +57,6 @@
     <t>Test Quote</t>
   </si>
   <si>
-    <t>U7BM9E</t>
-  </si>
-  <si>
     <t>72 - Special Negotiated Discount</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>MCCDiscAmt</t>
+  </si>
+  <si>
+    <t>G1S77A</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,19 +462,19 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K1" t="s">
         <v>9</v>
       </c>
       <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>19</v>
-      </c>
-      <c r="N1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -485,7 +485,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -494,31 +494,31 @@
         <v>-0.1</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
       </c>
       <c r="J2">
         <v>10</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L2">
         <v>72</v>
       </c>
       <c r="M2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" t="s">
         <v>21</v>
-      </c>
-      <c r="N2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>